<commit_message>
:construction: /teacher: submit point
</commit_message>
<xml_diff>
--- a/public/static/excels/lop-hoc-example.xlsx
+++ b/public/static/excels/lop-hoc-example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HoangNam\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\code\projects\b4e_new\school\frontend\public\static\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{98F28F70-318B-42A3-AD51-E7942FDEA6DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5DBB5E-DA03-4631-A032-CCC024F85808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6588259A-1796-4F86-8C8C-6B09693BB953}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>SSH1050</t>
   </si>
   <si>
-    <t>20161234, 201612345, 20161236, 20161237</t>
-  </si>
-  <si>
     <t>EM1170</t>
   </si>
   <si>
@@ -76,6 +73,9 @@
   </si>
   <si>
     <t>GV1237</t>
+  </si>
+  <si>
+    <t>20161234, 20161235, 20161236, 20161237</t>
   </si>
 </sst>
 </file>
@@ -430,7 +430,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" activeCellId="1" sqref="E4 E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,10 +466,10 @@
         <v>117123</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -477,16 +477,16 @@
         <v>20201</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>117124</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -494,16 +494,16 @@
         <v>20201</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>685542</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -511,16 +511,16 @@
         <v>20201</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5">
         <v>685547</v>
       </c>
       <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>